<commit_message>
main data changed and manipulated again, now data visualization started
</commit_message>
<xml_diff>
--- a/datastore manipulation/datastoresource/exsrk2019.xlsx
+++ b/datastore manipulation/datastoresource/exsrk2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emrec\Desktop\TUBITAK 22 DOSYASI\datastore manipulation\datastoresource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5C26BC-3D0C-44B4-8588-DAD767062BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E809E-1E75-4FB3-9DDA-88F4E1DB7D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,9 +597,6 @@
     <t xml:space="preserve">GÜBRE FABRİK. </t>
   </si>
   <si>
-    <t>GUSGR</t>
-  </si>
-  <si>
     <t xml:space="preserve">GÜNEŞ SİGORTA </t>
   </si>
   <si>
@@ -2058,9 +2055,6 @@
     <t xml:space="preserve">DOĞTAŞ KELEBEK MOBİLYA </t>
   </si>
   <si>
-    <t>DGKLB</t>
-  </si>
-  <si>
     <t xml:space="preserve">YEŞİL YAPI </t>
   </si>
   <si>
@@ -2509,6 +2503,12 @@
   </si>
   <si>
     <t>4ceyrek</t>
+  </si>
+  <si>
+    <t>DGNMO</t>
+  </si>
+  <si>
+    <t>TURSG</t>
   </si>
 </sst>
 </file>
@@ -11113,10 +11113,10 @@
   <dimension ref="A1:F418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H127" sqref="H127"/>
+      <selection pane="bottomRight" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11130,30 +11130,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>820</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>821</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>822</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>823</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>824</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>596</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>1</v>
@@ -11250,10 +11250,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>551</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
@@ -11290,10 +11290,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>1</v>
@@ -11370,10 +11370,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>1</v>
@@ -11390,10 +11390,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>593</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>594</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>1</v>
@@ -11430,10 +11430,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>383</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>384</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>1</v>
@@ -11470,10 +11470,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>0</v>
@@ -11510,10 +11510,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>645</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>646</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>1</v>
@@ -11570,10 +11570,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>386</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>0</v>
@@ -11710,10 +11710,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>417</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>1</v>
@@ -11830,10 +11830,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>0</v>
@@ -11890,10 +11890,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>443</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>444</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>1</v>
@@ -11950,10 +11950,10 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>1</v>
@@ -11970,10 +11970,10 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>1</v>
@@ -11990,10 +11990,10 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>1</v>
@@ -12010,10 +12010,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>552</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>553</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>1</v>
@@ -12030,10 +12030,10 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>387</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>388</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>1</v>
@@ -12050,10 +12050,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>1</v>
@@ -12070,10 +12070,10 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>1</v>
@@ -12090,10 +12090,10 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>1</v>
@@ -12110,10 +12110,10 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>1</v>
@@ -12130,10 +12130,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>1</v>
@@ -12250,10 +12250,10 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>1</v>
@@ -12310,10 +12310,10 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>0</v>
@@ -12330,10 +12330,10 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>1</v>
@@ -12370,10 +12370,10 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>513</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>514</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>1</v>
@@ -12410,10 +12410,10 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>418</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>419</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>1</v>
@@ -12430,10 +12430,10 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>421</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>1</v>
@@ -12450,10 +12450,10 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>500</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>501</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>1</v>
@@ -12570,10 +12570,10 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>1</v>
@@ -12670,10 +12670,10 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>1</v>
@@ -12690,10 +12690,10 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>0</v>
@@ -12710,10 +12710,10 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="9"/>
@@ -12746,10 +12746,10 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>1</v>
@@ -12906,10 +12906,10 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C90" s="13" t="s">
         <v>1</v>
@@ -12926,10 +12926,10 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>517</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>518</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>1</v>
@@ -12946,10 +12946,10 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>609</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>610</v>
       </c>
       <c r="C92" s="13" t="s">
         <v>1</v>
@@ -12966,10 +12966,10 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>422</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>423</v>
       </c>
       <c r="C93" s="13" t="s">
         <v>1</v>
@@ -12986,10 +12986,10 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>445</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>446</v>
       </c>
       <c r="C94" s="13" t="s">
         <v>1</v>
@@ -13026,10 +13026,10 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C96" s="13" t="s">
         <v>1</v>
@@ -13046,10 +13046,10 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C97" s="13"/>
       <c r="D97" s="9"/>
@@ -13140,10 +13140,10 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C102" s="13" t="s">
         <v>1</v>
@@ -13180,10 +13180,10 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>624</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>625</v>
       </c>
       <c r="C104" s="13" t="s">
         <v>1</v>
@@ -13220,10 +13220,10 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>1</v>
@@ -13280,10 +13280,10 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>425</v>
       </c>
       <c r="C109" s="13" t="s">
         <v>1</v>
@@ -13300,10 +13300,10 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C110" s="13" t="s">
         <v>1</v>
@@ -13340,10 +13340,10 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="2" t="s">
-        <v>675</v>
+        <v>824</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C112" s="13" t="s">
         <v>0</v>
@@ -13360,10 +13360,10 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="2" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>1</v>
@@ -13520,10 +13520,10 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>427</v>
       </c>
       <c r="C121" s="13" t="s">
         <v>1</v>
@@ -13560,10 +13560,10 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C123" s="13" t="s">
         <v>1</v>
@@ -13580,10 +13580,10 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" s="2" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C124" s="13" t="s">
         <v>1</v>
@@ -13600,10 +13600,10 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C125" s="13" t="s">
         <v>1</v>
@@ -13620,10 +13620,10 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>447</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>448</v>
       </c>
       <c r="C126" s="13" t="s">
         <v>1</v>
@@ -13640,10 +13640,10 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C127" s="13" t="s">
         <v>1</v>
@@ -13700,10 +13700,10 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>0</v>
@@ -13720,10 +13720,10 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="2" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C131" s="13" t="s">
         <v>0</v>
@@ -13840,10 +13840,10 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C137" s="13" t="s">
         <v>1</v>
@@ -13860,10 +13860,10 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B138" s="3" t="s">
         <v>538</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>539</v>
       </c>
       <c r="C138" s="13" t="s">
         <v>1</v>
@@ -13880,10 +13880,10 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>394</v>
       </c>
       <c r="C139" s="13" t="s">
         <v>1</v>
@@ -13900,10 +13900,10 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="2" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C140" s="13" t="s">
         <v>1</v>
@@ -13923,7 +13923,7 @@
         <v>161</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C141" s="13" t="s">
         <v>0</v>
@@ -13940,10 +13940,10 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C142" s="13" t="s">
         <v>1</v>
@@ -13960,10 +13960,10 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C143" s="13" t="s">
         <v>1</v>
@@ -13980,10 +13980,10 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B144" s="3" t="s">
         <v>584</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>585</v>
       </c>
       <c r="C144" s="13" t="s">
         <v>0</v>
@@ -14020,10 +14020,10 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C146" s="13" t="s">
         <v>1</v>
@@ -14060,10 +14060,10 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="2" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C148" s="13" t="s">
         <v>1</v>
@@ -14160,10 +14160,10 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B153" s="3" t="s">
         <v>395</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>396</v>
       </c>
       <c r="C153" s="13" t="s">
         <v>1</v>
@@ -14180,10 +14180,10 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B154" s="3" t="s">
         <v>472</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>473</v>
       </c>
       <c r="C154" s="13" t="s">
         <v>1</v>
@@ -14200,10 +14200,10 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C155" s="13" t="s">
         <v>1</v>
@@ -14220,10 +14220,10 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C156" s="13" t="s">
         <v>1</v>
@@ -14280,10 +14280,10 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C159" s="13" t="s">
         <v>1</v>
@@ -14360,10 +14360,10 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C163" s="13" t="s">
         <v>0</v>
@@ -14380,10 +14380,10 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C164" s="13" t="s">
         <v>1</v>
@@ -14440,10 +14440,10 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C167" s="13" t="s">
         <v>1</v>
@@ -14460,10 +14460,10 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B168" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="C168" s="13" t="s">
         <v>1</v>
@@ -14480,10 +14480,10 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C169" s="13" t="s">
         <v>1</v>
@@ -14500,10 +14500,10 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C170" s="13" t="s">
         <v>1</v>
@@ -14520,10 +14520,10 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B171" s="3" t="s">
         <v>648</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>649</v>
       </c>
       <c r="C171" s="13" t="s">
         <v>1</v>
@@ -14540,10 +14540,10 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B172" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="C172" s="13" t="s">
         <v>0</v>
@@ -14560,10 +14560,10 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C173" s="13" t="s">
         <v>1</v>
@@ -14580,10 +14580,10 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="C174" s="13" t="s">
         <v>0</v>
@@ -14600,10 +14600,10 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" s="2" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C175" s="13" t="s">
         <v>0</v>
@@ -14620,10 +14620,10 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C176" s="13" t="s">
         <v>1</v>
@@ -14640,10 +14640,10 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B177" s="3" t="s">
         <v>465</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>466</v>
       </c>
       <c r="C177" s="13" t="s">
         <v>1</v>
@@ -14660,10 +14660,10 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B178" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="C178" s="13" t="s">
         <v>1</v>
@@ -14680,10 +14680,10 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C179" s="13" t="s">
         <v>1</v>
@@ -14700,10 +14700,10 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B180" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="C180" s="13" t="s">
         <v>0</v>
@@ -14720,10 +14720,10 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C181" s="13" t="s">
         <v>0</v>
@@ -14740,10 +14740,10 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C182" s="13" t="s">
         <v>1</v>
@@ -14760,10 +14760,10 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B183" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="C183" s="13" t="s">
         <v>0</v>
@@ -14780,10 +14780,10 @@
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C184" s="13" t="s">
         <v>1</v>
@@ -14800,10 +14800,10 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B185" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="C185" s="13" t="s">
         <v>1</v>
@@ -14820,10 +14820,10 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C186" s="13" t="s">
         <v>0</v>
@@ -14840,10 +14840,10 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B187" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="C187" s="13" t="s">
         <v>1</v>
@@ -14860,10 +14860,10 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="C188" s="13" t="s">
         <v>1</v>
@@ -14880,10 +14880,10 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B189" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="C189" s="13" t="s">
         <v>0</v>
@@ -14900,10 +14900,10 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B190" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="C190" s="13" t="s">
         <v>1</v>
@@ -14920,10 +14920,10 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" s="2" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C191" s="13" t="s">
         <v>0</v>
@@ -14940,10 +14940,10 @@
     </row>
     <row r="192" spans="1:6">
       <c r="A192" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B192" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="C192" s="13" t="s">
         <v>1</v>
@@ -14960,10 +14960,10 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B193" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="C193" s="13" t="s">
         <v>1</v>
@@ -14980,10 +14980,10 @@
     </row>
     <row r="194" spans="1:6">
       <c r="A194" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>400</v>
       </c>
       <c r="C194" s="13" t="s">
         <v>0</v>
@@ -15000,10 +15000,10 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="C195" s="13" t="s">
         <v>1</v>
@@ -15020,10 +15020,10 @@
     </row>
     <row r="196" spans="1:6">
       <c r="A196" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C196" s="13" t="s">
         <v>1</v>
@@ -15040,10 +15040,10 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B197" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>429</v>
       </c>
       <c r="C197" s="13" t="s">
         <v>0</v>
@@ -15060,10 +15060,10 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B198" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="C198" s="13" t="s">
         <v>1</v>
@@ -15080,10 +15080,10 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="B199" s="3" t="s">
         <v>622</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>623</v>
       </c>
       <c r="C199" s="13" t="s">
         <v>1</v>
@@ -15100,10 +15100,10 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" s="2" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C200" s="13" t="s">
         <v>1</v>
@@ -15120,10 +15120,10 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C201" s="13" t="s">
         <v>1</v>
@@ -15140,10 +15140,10 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B202" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C202" s="13" t="s">
         <v>1</v>
@@ -15160,10 +15160,10 @@
     </row>
     <row r="203" spans="1:6">
       <c r="A203" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B203" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="C203" s="13" t="s">
         <v>1</v>
@@ -15180,10 +15180,10 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B204" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="C204" s="13" t="s">
         <v>1</v>
@@ -15200,10 +15200,10 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B205" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="C205" s="13" t="s">
         <v>0</v>
@@ -15220,10 +15220,10 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B206" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="C206" s="13" t="s">
         <v>1</v>
@@ -15240,10 +15240,10 @@
     </row>
     <row r="207" spans="1:6">
       <c r="A207" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="C207" s="13" t="s">
         <v>0</v>
@@ -15260,10 +15260,10 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B208" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="C208" s="13" t="s">
         <v>1</v>
@@ -15280,10 +15280,10 @@
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C209" s="13" t="s">
         <v>1</v>
@@ -15300,10 +15300,10 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B210" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="B210" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="C210" s="13" t="s">
         <v>0</v>
@@ -15320,10 +15320,10 @@
     </row>
     <row r="211" spans="1:6">
       <c r="A211" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B211" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="C211" s="13" t="s">
         <v>1</v>
@@ -15340,10 +15340,10 @@
     </row>
     <row r="212" spans="1:6">
       <c r="A212" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C212" s="13" t="s">
         <v>1</v>
@@ -15360,10 +15360,10 @@
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B213" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="B213" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="C213" s="13" t="s">
         <v>0</v>
@@ -15380,10 +15380,10 @@
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C214" s="13" t="s">
         <v>1</v>
@@ -15400,10 +15400,10 @@
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B215" s="3" t="s">
         <v>507</v>
-      </c>
-      <c r="B215" s="3" t="s">
-        <v>508</v>
       </c>
       <c r="C215" s="13" t="s">
         <v>1</v>
@@ -15420,10 +15420,10 @@
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B216" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="B216" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="C216" s="13" t="s">
         <v>1</v>
@@ -15440,10 +15440,10 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B217" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="B217" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="C217" s="13" t="s">
         <v>0</v>
@@ -15460,10 +15460,10 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B218" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="C218" s="13" t="s">
         <v>1</v>
@@ -15480,10 +15480,10 @@
     </row>
     <row r="219" spans="1:6">
       <c r="A219" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B219" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="B219" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="C219" s="13" t="s">
         <v>1</v>
@@ -15500,10 +15500,10 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C220" s="13" t="s">
         <v>0</v>
@@ -15520,10 +15520,10 @@
     </row>
     <row r="221" spans="1:6">
       <c r="A221" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C221" s="13" t="s">
         <v>0</v>
@@ -15540,10 +15540,10 @@
     </row>
     <row r="222" spans="1:6">
       <c r="A222" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B222" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="B222" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="C222" s="13" t="s">
         <v>0</v>
@@ -15560,10 +15560,10 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C223" s="13" t="s">
         <v>1</v>
@@ -15580,10 +15580,10 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B224" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="B224" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="C224" s="13" t="s">
         <v>1</v>
@@ -15600,10 +15600,10 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C225" s="13" t="s">
         <v>1</v>
@@ -15620,10 +15620,10 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C226" s="13" t="s">
         <v>1</v>
@@ -15640,10 +15640,10 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B227" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="B227" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="C227" s="13" t="s">
         <v>1</v>
@@ -15660,10 +15660,10 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C228" s="13" t="s">
         <v>1</v>
@@ -15680,10 +15680,10 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B229" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="B229" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="C229" s="13" t="s">
         <v>1</v>
@@ -15700,10 +15700,10 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B230" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="C230" s="13" t="s">
         <v>1</v>
@@ -15720,10 +15720,10 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C231" s="13" t="s">
         <v>1</v>
@@ -15740,10 +15740,10 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B232" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="B232" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="C232" s="13" t="s">
         <v>1</v>
@@ -15760,10 +15760,10 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B233" s="3" t="s">
         <v>449</v>
-      </c>
-      <c r="B233" s="3" t="s">
-        <v>450</v>
       </c>
       <c r="C233" s="13" t="s">
         <v>1</v>
@@ -15780,10 +15780,10 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B234" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B234" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="C234" s="13" t="s">
         <v>1</v>
@@ -15800,10 +15800,10 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C235" s="13" t="s">
         <v>1</v>
@@ -15820,10 +15820,10 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B236" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B236" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="C236" s="13" t="s">
         <v>1</v>
@@ -15840,10 +15840,10 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B237" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="B237" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="C237" s="13" t="s">
         <v>1</v>
@@ -15860,10 +15860,10 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C238" s="13" t="s">
         <v>1</v>
@@ -15880,10 +15880,10 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B239" s="3" t="s">
         <v>474</v>
-      </c>
-      <c r="B239" s="3" t="s">
-        <v>475</v>
       </c>
       <c r="C239" s="13" t="s">
         <v>1</v>
@@ -15900,10 +15900,10 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B240" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="B240" s="3" t="s">
-        <v>265</v>
       </c>
       <c r="C240" s="13" t="s">
         <v>1</v>
@@ -15920,10 +15920,10 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" s="2" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C241" s="13" t="s">
         <v>0</v>
@@ -15940,10 +15940,10 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>451</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>452</v>
       </c>
       <c r="C242" s="13" t="s">
         <v>1</v>
@@ -15960,10 +15960,10 @@
     </row>
     <row r="243" spans="1:6">
       <c r="A243" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="C243" s="13" t="s">
         <v>1</v>
@@ -15980,10 +15980,10 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="2" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C244" s="13" t="s">
         <v>0</v>
@@ -16000,10 +16000,10 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C245" s="13"/>
       <c r="D245" s="9" t="s">
@@ -16018,10 +16018,10 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B246" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="C246" s="13" t="s">
         <v>1</v>
@@ -16038,10 +16038,10 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B247" s="3" t="s">
         <v>431</v>
-      </c>
-      <c r="B247" s="3" t="s">
-        <v>432</v>
       </c>
       <c r="C247" s="13" t="s">
         <v>1</v>
@@ -16058,10 +16058,10 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C248" s="13" t="s">
         <v>0</v>
@@ -16078,10 +16078,10 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B249" s="3" t="s">
         <v>531</v>
-      </c>
-      <c r="B249" s="3" t="s">
-        <v>532</v>
       </c>
       <c r="C249" s="13" t="s">
         <v>1</v>
@@ -16098,10 +16098,10 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="2" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C250" s="13" t="s">
         <v>1</v>
@@ -16118,10 +16118,10 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C251" s="13" t="s">
         <v>1</v>
@@ -16138,10 +16138,10 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C252" s="13" t="s">
         <v>1</v>
@@ -16158,10 +16158,10 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B253" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="B253" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="C253" s="13" t="s">
         <v>0</v>
@@ -16178,10 +16178,10 @@
     </row>
     <row r="254" spans="1:6">
       <c r="A254" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="C254" s="13" t="s">
         <v>1</v>
@@ -16198,10 +16198,10 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C255" s="13" t="s">
         <v>1</v>
@@ -16218,10 +16218,10 @@
     </row>
     <row r="256" spans="1:6">
       <c r="A256" s="2" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C256" s="13"/>
       <c r="D256" s="9"/>
@@ -16232,10 +16232,10 @@
     </row>
     <row r="257" spans="1:6">
       <c r="A257" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B257" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="B257" s="3" t="s">
-        <v>276</v>
       </c>
       <c r="C257" s="13" t="s">
         <v>0</v>
@@ -16252,10 +16252,10 @@
     </row>
     <row r="258" spans="1:6">
       <c r="A258" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B258" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="B258" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="C258" s="13" t="s">
         <v>0</v>
@@ -16272,10 +16272,10 @@
     </row>
     <row r="259" spans="1:6">
       <c r="A259" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C259" s="13" t="s">
         <v>1</v>
@@ -16292,10 +16292,10 @@
     </row>
     <row r="260" spans="1:6">
       <c r="A260" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="C260" s="13" t="s">
         <v>1</v>
@@ -16312,10 +16312,10 @@
     </row>
     <row r="261" spans="1:6">
       <c r="A261" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>402</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>403</v>
       </c>
       <c r="C261" s="13" t="s">
         <v>1</v>
@@ -16332,10 +16332,10 @@
     </row>
     <row r="262" spans="1:6">
       <c r="A262" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="B262" s="3" t="s">
         <v>658</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>659</v>
       </c>
       <c r="C262" s="13" t="s">
         <v>0</v>
@@ -16352,10 +16352,10 @@
     </row>
     <row r="263" spans="1:6">
       <c r="A263" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C263" s="13" t="s">
         <v>1</v>
@@ -16372,10 +16372,10 @@
     </row>
     <row r="264" spans="1:6">
       <c r="A264" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>568</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>569</v>
       </c>
       <c r="C264" s="13" t="s">
         <v>1</v>
@@ -16392,10 +16392,10 @@
     </row>
     <row r="265" spans="1:6">
       <c r="A265" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B265" s="3" t="s">
         <v>565</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>566</v>
       </c>
       <c r="C265" s="13" t="s">
         <v>1</v>
@@ -16412,10 +16412,10 @@
     </row>
     <row r="266" spans="1:6">
       <c r="A266" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B266" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="C266" s="13" t="s">
         <v>0</v>
@@ -16432,10 +16432,10 @@
     </row>
     <row r="267" spans="1:6">
       <c r="A267" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B267" s="3" t="s">
         <v>404</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>405</v>
       </c>
       <c r="C267" s="13" t="s">
         <v>1</v>
@@ -16452,10 +16452,10 @@
     </row>
     <row r="268" spans="1:6">
       <c r="A268" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B268" s="3" t="s">
         <v>563</v>
-      </c>
-      <c r="B268" s="3" t="s">
-        <v>564</v>
       </c>
       <c r="C268" s="13" t="s">
         <v>1</v>
@@ -16472,10 +16472,10 @@
     </row>
     <row r="269" spans="1:6">
       <c r="A269" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C269" s="13" t="s">
         <v>1</v>
@@ -16492,10 +16492,10 @@
     </row>
     <row r="270" spans="1:6">
       <c r="A270" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C270" s="13" t="s">
         <v>1</v>
@@ -16512,10 +16512,10 @@
     </row>
     <row r="271" spans="1:6">
       <c r="A271" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B271" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>534</v>
       </c>
       <c r="C271" s="13" t="s">
         <v>1</v>
@@ -16532,10 +16532,10 @@
     </row>
     <row r="272" spans="1:6">
       <c r="A272" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>406</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>407</v>
       </c>
       <c r="C272" s="13" t="s">
         <v>1</v>
@@ -16552,10 +16552,10 @@
     </row>
     <row r="273" spans="1:6">
       <c r="A273" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B273" s="3" t="s">
         <v>660</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>661</v>
       </c>
       <c r="C273" s="13" t="s">
         <v>1</v>
@@ -16572,10 +16572,10 @@
     </row>
     <row r="274" spans="1:6">
       <c r="A274" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C274" s="13" t="s">
         <v>0</v>
@@ -16592,10 +16592,10 @@
     </row>
     <row r="275" spans="1:6">
       <c r="A275" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B275" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="C275" s="13" t="s">
         <v>0</v>
@@ -16612,10 +16612,10 @@
     </row>
     <row r="276" spans="1:6">
       <c r="A276" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B276" s="8" t="s">
         <v>654</v>
-      </c>
-      <c r="B276" s="8" t="s">
-        <v>655</v>
       </c>
       <c r="C276" s="13" t="s">
         <v>0</v>
@@ -16632,10 +16632,10 @@
     </row>
     <row r="277" spans="1:6">
       <c r="A277" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="C277" s="13" t="s">
         <v>1</v>
@@ -16652,10 +16652,10 @@
     </row>
     <row r="278" spans="1:6">
       <c r="A278" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B278" s="3" t="s">
         <v>408</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>409</v>
       </c>
       <c r="C278" s="13" t="s">
         <v>1</v>
@@ -16672,10 +16672,10 @@
     </row>
     <row r="279" spans="1:6">
       <c r="A279" s="2" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C279" s="13" t="s">
         <v>1</v>
@@ -16692,10 +16692,10 @@
     </row>
     <row r="280" spans="1:6">
       <c r="A280" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B280" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="B280" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="C280" s="13" t="s">
         <v>0</v>
@@ -16712,10 +16712,10 @@
     </row>
     <row r="281" spans="1:6">
       <c r="A281" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B281" s="3" t="s">
         <v>433</v>
-      </c>
-      <c r="B281" s="3" t="s">
-        <v>434</v>
       </c>
       <c r="C281" s="13" t="s">
         <v>1</v>
@@ -16732,10 +16732,10 @@
     </row>
     <row r="282" spans="1:6">
       <c r="A282" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B282" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="B282" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="C282" s="13" t="s">
         <v>1</v>
@@ -16752,10 +16752,10 @@
     </row>
     <row r="283" spans="1:6">
       <c r="A283" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B283" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="B283" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="C283" s="13" t="s">
         <v>1</v>
@@ -16772,10 +16772,10 @@
     </row>
     <row r="284" spans="1:6">
       <c r="A284" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B284" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="B284" s="3" t="s">
-        <v>295</v>
       </c>
       <c r="C284" s="13" t="s">
         <v>1</v>
@@ -16792,10 +16792,10 @@
     </row>
     <row r="285" spans="1:6">
       <c r="A285" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B285" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="B285" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="C285" s="13" t="s">
         <v>1</v>
@@ -16812,10 +16812,10 @@
     </row>
     <row r="286" spans="1:6">
       <c r="A286" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C286" s="13" t="s">
         <v>0</v>
@@ -16832,10 +16832,10 @@
     </row>
     <row r="287" spans="1:6">
       <c r="A287" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C287" s="13" t="s">
         <v>1</v>
@@ -16852,10 +16852,10 @@
     </row>
     <row r="288" spans="1:6">
       <c r="A288" s="2" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C288" s="13" t="s">
         <v>1</v>
@@ -16872,10 +16872,10 @@
     </row>
     <row r="289" spans="1:6">
       <c r="A289" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B289" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="B289" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="C289" s="13" t="s">
         <v>1</v>
@@ -16892,10 +16892,10 @@
     </row>
     <row r="290" spans="1:6">
       <c r="A290" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>469</v>
-      </c>
-      <c r="B290" s="3" t="s">
-        <v>470</v>
       </c>
       <c r="C290" s="13" t="s">
         <v>1</v>
@@ -16912,10 +16912,10 @@
     </row>
     <row r="291" spans="1:6">
       <c r="A291" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>301</v>
       </c>
       <c r="C291" s="13" t="s">
         <v>1</v>
@@ -16932,10 +16932,10 @@
     </row>
     <row r="292" spans="1:6">
       <c r="A292" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>656</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>657</v>
       </c>
       <c r="C292" s="13" t="s">
         <v>1</v>
@@ -16952,10 +16952,10 @@
     </row>
     <row r="293" spans="1:6">
       <c r="A293" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C293" s="13" t="s">
         <v>1</v>
@@ -16972,10 +16972,10 @@
     </row>
     <row r="294" spans="1:6">
       <c r="A294" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C294" s="13" t="s">
         <v>1</v>
@@ -16992,10 +16992,10 @@
     </row>
     <row r="295" spans="1:6">
       <c r="A295" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C295" s="13" t="s">
         <v>1</v>
@@ -17012,10 +17012,10 @@
     </row>
     <row r="296" spans="1:6">
       <c r="A296" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B296" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="B296" s="3" t="s">
-        <v>303</v>
       </c>
       <c r="C296" s="13" t="s">
         <v>0</v>
@@ -17032,10 +17032,10 @@
     </row>
     <row r="297" spans="1:6">
       <c r="A297" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C297" s="13" t="s">
         <v>1</v>
@@ -17052,10 +17052,10 @@
     </row>
     <row r="298" spans="1:6">
       <c r="A298" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C298" s="13" t="s">
         <v>1</v>
@@ -17072,10 +17072,10 @@
     </row>
     <row r="299" spans="1:6">
       <c r="A299" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C299" s="13" t="s">
         <v>1</v>
@@ -17092,10 +17092,10 @@
     </row>
     <row r="300" spans="1:6">
       <c r="A300" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B300" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="B300" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="C300" s="13" t="s">
         <v>1</v>
@@ -17112,10 +17112,10 @@
     </row>
     <row r="301" spans="1:6">
       <c r="A301" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B301" s="3" t="s">
         <v>521</v>
-      </c>
-      <c r="B301" s="3" t="s">
-        <v>522</v>
       </c>
       <c r="C301" s="13" t="s">
         <v>1</v>
@@ -17132,10 +17132,10 @@
     </row>
     <row r="302" spans="1:6">
       <c r="A302" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="B302" s="3" t="s">
         <v>664</v>
-      </c>
-      <c r="B302" s="3" t="s">
-        <v>665</v>
       </c>
       <c r="C302" s="13" t="s">
         <v>1</v>
@@ -17152,10 +17152,10 @@
     </row>
     <row r="303" spans="1:6">
       <c r="A303" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C303" s="13" t="s">
         <v>1</v>
@@ -17172,10 +17172,10 @@
     </row>
     <row r="304" spans="1:6">
       <c r="A304" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B304" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="B304" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="C304" s="13" t="s">
         <v>1</v>
@@ -17195,7 +17195,7 @@
         <v>10</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C305" s="13" t="s">
         <v>0</v>
@@ -17212,10 +17212,10 @@
     </row>
     <row r="306" spans="1:6">
       <c r="A306" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B306" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="B306" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="C306" s="13" t="s">
         <v>1</v>
@@ -17232,10 +17232,10 @@
     </row>
     <row r="307" spans="1:6">
       <c r="A307" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B307" s="3" t="s">
         <v>453</v>
-      </c>
-      <c r="B307" s="3" t="s">
-        <v>454</v>
       </c>
       <c r="C307" s="13" t="s">
         <v>1</v>
@@ -17252,10 +17252,10 @@
     </row>
     <row r="308" spans="1:6">
       <c r="A308" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C308" s="13" t="s">
         <v>1</v>
@@ -17272,10 +17272,10 @@
     </row>
     <row r="309" spans="1:6">
       <c r="A309" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B309" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="B309" s="3" t="s">
-        <v>311</v>
       </c>
       <c r="C309" s="13" t="s">
         <v>1</v>
@@ -17292,10 +17292,10 @@
     </row>
     <row r="310" spans="1:6">
       <c r="A310" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B310" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="B310" s="3" t="s">
-        <v>436</v>
       </c>
       <c r="C310" s="13" t="s">
         <v>1</v>
@@ -17312,10 +17312,10 @@
     </row>
     <row r="311" spans="1:6">
       <c r="A311" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C311" s="13"/>
       <c r="D311" s="9"/>
@@ -17328,10 +17328,10 @@
     </row>
     <row r="312" spans="1:6">
       <c r="A312" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B312" s="3" t="s">
         <v>410</v>
-      </c>
-      <c r="B312" s="3" t="s">
-        <v>411</v>
       </c>
       <c r="C312" s="13" t="s">
         <v>1</v>
@@ -17348,10 +17348,10 @@
     </row>
     <row r="313" spans="1:6">
       <c r="A313" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B313" s="3" t="s">
         <v>312</v>
-      </c>
-      <c r="B313" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="C313" s="13" t="s">
         <v>0</v>
@@ -17368,10 +17368,10 @@
     </row>
     <row r="314" spans="1:6">
       <c r="A314" s="2" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C314" s="13" t="s">
         <v>0</v>
@@ -17388,10 +17388,10 @@
     </row>
     <row r="315" spans="1:6">
       <c r="A315" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B315" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="B315" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="C315" s="13" t="s">
         <v>1</v>
@@ -17408,10 +17408,10 @@
     </row>
     <row r="316" spans="1:6">
       <c r="A316" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B316" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="B316" s="3" t="s">
-        <v>438</v>
       </c>
       <c r="C316" s="13" t="s">
         <v>1</v>
@@ -17428,10 +17428,10 @@
     </row>
     <row r="317" spans="1:6">
       <c r="A317" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B317" s="3" t="s">
         <v>439</v>
-      </c>
-      <c r="B317" s="3" t="s">
-        <v>440</v>
       </c>
       <c r="C317" s="13" t="s">
         <v>1</v>
@@ -17448,10 +17448,10 @@
     </row>
     <row r="318" spans="1:6">
       <c r="A318" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B318" s="3" t="s">
         <v>441</v>
-      </c>
-      <c r="B318" s="3" t="s">
-        <v>442</v>
       </c>
       <c r="C318" s="13" t="s">
         <v>1</v>
@@ -17468,10 +17468,10 @@
     </row>
     <row r="319" spans="1:6">
       <c r="A319" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B319" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="B319" s="3" t="s">
-        <v>317</v>
       </c>
       <c r="C319" s="13" t="s">
         <v>0</v>
@@ -17488,10 +17488,10 @@
     </row>
     <row r="320" spans="1:6">
       <c r="A320" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B320" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="B320" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="C320" s="13" t="s">
         <v>0</v>
@@ -17508,10 +17508,10 @@
     </row>
     <row r="321" spans="1:6">
       <c r="A321" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B321" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="B321" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="C321" s="13" t="s">
         <v>0</v>
@@ -17528,10 +17528,10 @@
     </row>
     <row r="322" spans="1:6">
       <c r="A322" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C322" s="13" t="s">
         <v>1</v>
@@ -17548,10 +17548,10 @@
     </row>
     <row r="323" spans="1:6">
       <c r="A323" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C323" s="13" t="s">
         <v>1</v>
@@ -17568,10 +17568,10 @@
     </row>
     <row r="324" spans="1:6">
       <c r="A324" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B324" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="B324" s="3" t="s">
-        <v>337</v>
       </c>
       <c r="C324" s="13" t="s">
         <v>0</v>
@@ -17588,10 +17588,10 @@
     </row>
     <row r="325" spans="1:6">
       <c r="A325" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B325" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="B325" s="3" t="s">
-        <v>340</v>
       </c>
       <c r="C325" s="13" t="s">
         <v>1</v>
@@ -17608,10 +17608,10 @@
     </row>
     <row r="326" spans="1:6">
       <c r="A326" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C326" s="13" t="s">
         <v>0</v>
@@ -17628,10 +17628,10 @@
     </row>
     <row r="327" spans="1:6">
       <c r="A327" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B327" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="B327" s="3" t="s">
-        <v>324</v>
       </c>
       <c r="C327" s="13" t="s">
         <v>0</v>
@@ -17648,10 +17648,10 @@
     </row>
     <row r="328" spans="1:6">
       <c r="A328" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B328" s="3" t="s">
         <v>579</v>
-      </c>
-      <c r="B328" s="3" t="s">
-        <v>580</v>
       </c>
       <c r="C328" s="13" t="s">
         <v>1</v>
@@ -17668,10 +17668,10 @@
     </row>
     <row r="329" spans="1:6">
       <c r="A329" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B329" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="B329" s="3" t="s">
-        <v>326</v>
       </c>
       <c r="C329" s="13" t="s">
         <v>1</v>
@@ -17688,10 +17688,10 @@
     </row>
     <row r="330" spans="1:6">
       <c r="A330" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B330" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="B330" s="3" t="s">
-        <v>328</v>
       </c>
       <c r="C330" s="13" t="s">
         <v>0</v>
@@ -17708,10 +17708,10 @@
     </row>
     <row r="331" spans="1:6">
       <c r="A331" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B331" s="3" t="s">
         <v>570</v>
-      </c>
-      <c r="B331" s="3" t="s">
-        <v>571</v>
       </c>
       <c r="C331" s="13" t="s">
         <v>1</v>
@@ -17728,10 +17728,10 @@
     </row>
     <row r="332" spans="1:6">
       <c r="A332" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C332" s="13" t="s">
         <v>1</v>
@@ -17748,10 +17748,10 @@
     </row>
     <row r="333" spans="1:6">
       <c r="A333" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B333" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="B333" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="C333" s="13" t="s">
         <v>0</v>
@@ -17768,10 +17768,10 @@
     </row>
     <row r="334" spans="1:6">
       <c r="A334" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C334" s="13" t="s">
         <v>1</v>
@@ -17788,10 +17788,10 @@
     </row>
     <row r="335" spans="1:6">
       <c r="A335" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B335" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="B335" s="3" t="s">
-        <v>333</v>
       </c>
       <c r="C335" s="13" t="s">
         <v>1</v>
@@ -17808,10 +17808,10 @@
     </row>
     <row r="336" spans="1:6">
       <c r="A336" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B336" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="B336" s="3" t="s">
-        <v>335</v>
       </c>
       <c r="C336" s="13" t="s">
         <v>0</v>
@@ -17828,10 +17828,10 @@
     </row>
     <row r="337" spans="1:6">
       <c r="A337" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C337" s="13" t="s">
         <v>1</v>
@@ -17848,10 +17848,10 @@
     </row>
     <row r="338" spans="1:6">
       <c r="A338" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C338" s="13" t="s">
         <v>1</v>
@@ -17868,10 +17868,10 @@
     </row>
     <row r="339" spans="1:6">
       <c r="A339" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B339" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="B339" s="3" t="s">
-        <v>342</v>
       </c>
       <c r="C339" s="13" t="s">
         <v>1</v>
@@ -17888,10 +17888,10 @@
     </row>
     <row r="340" spans="1:6">
       <c r="A340" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B340" s="3" t="s">
         <v>343</v>
-      </c>
-      <c r="B340" s="3" t="s">
-        <v>344</v>
       </c>
       <c r="C340" s="13" t="s">
         <v>1</v>
@@ -17908,10 +17908,10 @@
     </row>
     <row r="341" spans="1:6">
       <c r="A341" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B341" s="3" t="s">
         <v>345</v>
-      </c>
-      <c r="B341" s="3" t="s">
-        <v>346</v>
       </c>
       <c r="C341" s="13" t="s">
         <v>0</v>
@@ -17928,10 +17928,10 @@
     </row>
     <row r="342" spans="1:6">
       <c r="A342" s="2" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C342" s="13" t="s">
         <v>1</v>
@@ -17948,10 +17948,10 @@
     </row>
     <row r="343" spans="1:6">
       <c r="A343" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B343" s="3" t="s">
         <v>642</v>
-      </c>
-      <c r="B343" s="3" t="s">
-        <v>643</v>
       </c>
       <c r="C343" s="13" t="s">
         <v>0</v>
@@ -17968,10 +17968,10 @@
     </row>
     <row r="344" spans="1:6">
       <c r="A344" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B344" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="B344" s="3" t="s">
-        <v>348</v>
       </c>
       <c r="C344" s="13" t="s">
         <v>0</v>
@@ -17988,10 +17988,10 @@
     </row>
     <row r="345" spans="1:6">
       <c r="A345" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B345" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="B345" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="C345" s="13" t="s">
         <v>0</v>
@@ -18008,10 +18008,10 @@
     </row>
     <row r="346" spans="1:6">
       <c r="A346" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B346" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="B346" s="3" t="s">
-        <v>352</v>
       </c>
       <c r="C346" s="13" t="s">
         <v>1</v>
@@ -18028,10 +18028,10 @@
     </row>
     <row r="347" spans="1:6">
       <c r="A347" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B347" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="B347" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="C347" s="13" t="s">
         <v>0</v>
@@ -18048,10 +18048,10 @@
     </row>
     <row r="348" spans="1:6">
       <c r="A348" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B348" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="B348" s="3" t="s">
-        <v>356</v>
       </c>
       <c r="C348" s="13" t="s">
         <v>0</v>
@@ -18068,10 +18068,10 @@
     </row>
     <row r="349" spans="1:6">
       <c r="A349" s="2" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C349" s="13" t="s">
         <v>1</v>
@@ -18088,10 +18088,10 @@
     </row>
     <row r="350" spans="1:6">
       <c r="A350" s="2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C350" s="13" t="s">
         <v>1</v>
@@ -18108,10 +18108,10 @@
     </row>
     <row r="351" spans="1:6">
       <c r="A351" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C351" s="13" t="s">
         <v>1</v>
@@ -18128,10 +18128,10 @@
     </row>
     <row r="352" spans="1:6">
       <c r="A352" s="2" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C352" s="13" t="s">
         <v>1</v>
@@ -18148,10 +18148,10 @@
     </row>
     <row r="353" spans="1:6">
       <c r="A353" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="B353" s="3" t="s">
         <v>616</v>
-      </c>
-      <c r="B353" s="3" t="s">
-        <v>617</v>
       </c>
       <c r="C353" s="13" t="s">
         <v>1</v>
@@ -18168,10 +18168,10 @@
     </row>
     <row r="354" spans="1:6">
       <c r="A354" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B354" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="B354" s="3" t="s">
-        <v>358</v>
       </c>
       <c r="C354" s="13" t="s">
         <v>1</v>
@@ -18188,10 +18188,10 @@
     </row>
     <row r="355" spans="1:6">
       <c r="A355" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C355" s="13" t="s">
         <v>1</v>
@@ -18208,10 +18208,10 @@
     </row>
     <row r="356" spans="1:6">
       <c r="A356" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B356" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="B356" s="3" t="s">
-        <v>360</v>
       </c>
       <c r="C356" s="13" t="s">
         <v>0</v>
@@ -18228,10 +18228,10 @@
     </row>
     <row r="357" spans="1:6">
       <c r="A357" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B357" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="B357" s="3" t="s">
-        <v>362</v>
       </c>
       <c r="C357" s="13" t="s">
         <v>1</v>
@@ -18248,10 +18248,10 @@
     </row>
     <row r="358" spans="1:6">
       <c r="A358" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B358" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="B358" s="3" t="s">
-        <v>364</v>
       </c>
       <c r="C358" s="13" t="s">
         <v>1</v>
@@ -18268,10 +18268,10 @@
     </row>
     <row r="359" spans="1:6">
       <c r="A359" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B359" s="3" t="s">
         <v>412</v>
-      </c>
-      <c r="B359" s="3" t="s">
-        <v>413</v>
       </c>
       <c r="C359" s="13" t="s">
         <v>1</v>
@@ -18288,10 +18288,10 @@
     </row>
     <row r="360" spans="1:6">
       <c r="A360" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C360" s="13" t="s">
         <v>1</v>
@@ -18308,10 +18308,10 @@
     </row>
     <row r="361" spans="1:6">
       <c r="A361" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B361" s="3" t="s">
         <v>365</v>
-      </c>
-      <c r="B361" s="3" t="s">
-        <v>366</v>
       </c>
       <c r="C361" s="13" t="s">
         <v>0</v>
@@ -18328,10 +18328,10 @@
     </row>
     <row r="362" spans="1:6">
       <c r="A362" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B362" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="B362" s="3" t="s">
-        <v>368</v>
       </c>
       <c r="C362" s="13" t="s">
         <v>1</v>
@@ -18348,10 +18348,10 @@
     </row>
     <row r="363" spans="1:6">
       <c r="A363" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C363" s="13" t="s">
         <v>0</v>
@@ -18368,10 +18368,10 @@
     </row>
     <row r="364" spans="1:6">
       <c r="A364" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C364" s="13" t="s">
         <v>1</v>
@@ -18388,10 +18388,10 @@
     </row>
     <row r="365" spans="1:6">
       <c r="A365" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B365" s="3" t="s">
         <v>369</v>
-      </c>
-      <c r="B365" s="3" t="s">
-        <v>370</v>
       </c>
       <c r="C365" s="13" t="s">
         <v>0</v>
@@ -18408,10 +18408,10 @@
     </row>
     <row r="366" spans="1:6">
       <c r="A366" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B366" s="3" t="s">
         <v>371</v>
-      </c>
-      <c r="B366" s="3" t="s">
-        <v>372</v>
       </c>
       <c r="C366" s="13" t="s">
         <v>1</v>
@@ -18428,10 +18428,10 @@
     </row>
     <row r="367" spans="1:6">
       <c r="A367" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B367" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="B367" s="3" t="s">
-        <v>374</v>
       </c>
       <c r="C367" s="13" t="s">
         <v>1</v>
@@ -18448,10 +18448,10 @@
     </row>
     <row r="368" spans="1:6">
       <c r="A368" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B368" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="B368" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="C368" s="13" t="s">
         <v>1</v>
@@ -18468,10 +18468,10 @@
     </row>
     <row r="369" spans="1:6">
       <c r="A369" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B369" s="3" t="s">
         <v>375</v>
-      </c>
-      <c r="B369" s="3" t="s">
-        <v>376</v>
       </c>
       <c r="C369" s="13" t="s">
         <v>0</v>
@@ -18488,10 +18488,10 @@
     </row>
     <row r="370" spans="1:6">
       <c r="A370" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B370" s="3" t="s">
         <v>511</v>
-      </c>
-      <c r="B370" s="3" t="s">
-        <v>512</v>
       </c>
       <c r="C370" s="13" t="s">
         <v>1</v>
@@ -18508,10 +18508,10 @@
     </row>
     <row r="371" spans="1:6">
       <c r="A371" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B371" s="3" t="s">
         <v>377</v>
-      </c>
-      <c r="B371" s="3" t="s">
-        <v>378</v>
       </c>
       <c r="C371" s="13" t="s">
         <v>0</v>
@@ -18528,10 +18528,10 @@
     </row>
     <row r="372" spans="1:6">
       <c r="A372" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="B372" s="3" t="s">
         <v>668</v>
-      </c>
-      <c r="B372" s="3" t="s">
-        <v>669</v>
       </c>
       <c r="C372" s="13" t="s">
         <v>1</v>
@@ -18548,10 +18548,10 @@
     </row>
     <row r="373" spans="1:6">
       <c r="A373" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C373" s="13" t="s">
         <v>1</v>
@@ -18568,10 +18568,10 @@
     </row>
     <row r="374" spans="1:6">
       <c r="A374" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C374" s="13" t="s">
         <v>1</v>
@@ -18588,10 +18588,10 @@
     </row>
     <row r="375" spans="1:6">
       <c r="A375" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C375" s="13" t="s">
         <v>1</v>
@@ -18608,10 +18608,10 @@
     </row>
     <row r="376" spans="1:6">
       <c r="A376" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B376" s="3" t="s">
         <v>379</v>
-      </c>
-      <c r="B376" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="C376" s="13" t="s">
         <v>1</v>
@@ -18628,10 +18628,10 @@
     </row>
     <row r="377" spans="1:6">
       <c r="A377" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B377" s="3" t="s">
         <v>381</v>
-      </c>
-      <c r="B377" s="3" t="s">
-        <v>382</v>
       </c>
       <c r="C377" s="13" t="s">
         <v>0</v>
@@ -18648,10 +18648,10 @@
     </row>
     <row r="378" spans="1:6">
       <c r="A378" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C378" s="13" t="s">
         <v>1</v>
@@ -18668,10 +18668,10 @@
     </row>
     <row r="379" spans="1:6">
       <c r="A379" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C379" s="13" t="s">
         <v>1</v>
@@ -18688,10 +18688,10 @@
     </row>
     <row r="380" spans="1:6">
       <c r="A380" s="2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C380" s="13" t="s">
         <v>1</v>
@@ -18708,10 +18708,10 @@
     </row>
     <row r="381" spans="1:6">
       <c r="A381" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="B381" s="3" t="s">
         <v>613</v>
-      </c>
-      <c r="B381" s="3" t="s">
-        <v>614</v>
       </c>
       <c r="C381" s="13" t="s">
         <v>1</v>
@@ -18728,10 +18728,10 @@
     </row>
     <row r="382" spans="1:6">
       <c r="A382" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C382" s="13" t="s">
         <v>1</v>
@@ -18748,10 +18748,10 @@
     </row>
     <row r="383" spans="1:6">
       <c r="A383" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C383" s="13" t="s">
         <v>1</v>
@@ -18768,10 +18768,10 @@
     </row>
     <row r="384" spans="1:6">
       <c r="A384" s="2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C384" s="13" t="s">
         <v>1</v>
@@ -18788,10 +18788,10 @@
     </row>
     <row r="385" spans="1:6">
       <c r="A385" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C385" s="13" t="s">
         <v>1</v>
@@ -18808,10 +18808,10 @@
     </row>
     <row r="386" spans="1:6">
       <c r="A386" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C386" s="13" t="s">
         <v>1</v>
@@ -18828,10 +18828,10 @@
     </row>
     <row r="387" spans="1:6">
       <c r="A387" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C387" s="13" t="s">
         <v>1</v>
@@ -18848,10 +18848,10 @@
     </row>
     <row r="388" spans="1:6">
       <c r="A388" s="2" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C388" s="13" t="s">
         <v>1</v>
@@ -18868,10 +18868,10 @@
     </row>
     <row r="389" spans="1:6">
       <c r="A389" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C389" s="13" t="s">
         <v>1</v>
@@ -18888,10 +18888,10 @@
     </row>
     <row r="390" spans="1:6">
       <c r="A390" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="B390" s="3" t="s">
         <v>670</v>
-      </c>
-      <c r="B390" s="3" t="s">
-        <v>671</v>
       </c>
       <c r="C390" s="13" t="s">
         <v>1</v>
@@ -18908,10 +18908,10 @@
     </row>
     <row r="391" spans="1:6">
       <c r="A391" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B391" s="3" t="s">
         <v>672</v>
-      </c>
-      <c r="B391" s="3" t="s">
-        <v>673</v>
       </c>
       <c r="C391" s="13" t="s">
         <v>1</v>
@@ -18928,10 +18928,10 @@
     </row>
     <row r="392" spans="1:6">
       <c r="A392" s="2" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C392" s="13" t="s">
         <v>1</v>
@@ -18948,10 +18948,10 @@
     </row>
     <row r="393" spans="1:6">
       <c r="A393" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B393" s="3" t="s">
         <v>662</v>
-      </c>
-      <c r="B393" s="3" t="s">
-        <v>663</v>
       </c>
       <c r="C393" s="13" t="s">
         <v>1</v>
@@ -18968,10 +18968,10 @@
     </row>
     <row r="394" spans="1:6">
       <c r="A394" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="B394" s="3" t="s">
         <v>632</v>
-      </c>
-      <c r="B394" s="3" t="s">
-        <v>633</v>
       </c>
       <c r="C394" s="13" t="s">
         <v>1</v>
@@ -18988,10 +18988,10 @@
     </row>
     <row r="395" spans="1:6">
       <c r="A395" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B395" s="3" t="s">
         <v>541</v>
-      </c>
-      <c r="B395" s="3" t="s">
-        <v>542</v>
       </c>
       <c r="C395" s="13" t="s">
         <v>1</v>
@@ -19008,10 +19008,10 @@
     </row>
     <row r="396" spans="1:6">
       <c r="A396" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C396" s="13" t="s">
         <v>1</v>
@@ -19028,10 +19028,10 @@
     </row>
     <row r="397" spans="1:6">
       <c r="A397" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C397" s="13" t="s">
         <v>1</v>
@@ -19048,10 +19048,10 @@
     </row>
     <row r="398" spans="1:6">
       <c r="A398" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B398" s="3" t="s">
         <v>620</v>
-      </c>
-      <c r="B398" s="3" t="s">
-        <v>621</v>
       </c>
       <c r="C398" s="13" t="s">
         <v>1</v>
@@ -19068,10 +19068,10 @@
     </row>
     <row r="399" spans="1:6">
       <c r="A399" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B399" s="3" t="s">
         <v>603</v>
-      </c>
-      <c r="B399" s="3" t="s">
-        <v>604</v>
       </c>
       <c r="C399" s="13" t="s">
         <v>1</v>
@@ -19088,10 +19088,10 @@
     </row>
     <row r="400" spans="1:6">
       <c r="A400" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="B400" s="3" t="s">
         <v>574</v>
-      </c>
-      <c r="B400" s="3" t="s">
-        <v>575</v>
       </c>
       <c r="C400" s="13" t="s">
         <v>1</v>
@@ -19108,10 +19108,10 @@
     </row>
     <row r="401" spans="1:6">
       <c r="A401" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B401" s="3" t="s">
         <v>634</v>
-      </c>
-      <c r="B401" s="3" t="s">
-        <v>635</v>
       </c>
       <c r="C401" s="13" t="s">
         <v>1</v>
@@ -19128,10 +19128,10 @@
     </row>
     <row r="402" spans="1:6">
       <c r="A402" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="B402" s="3" t="s">
         <v>636</v>
-      </c>
-      <c r="B402" s="3" t="s">
-        <v>637</v>
       </c>
       <c r="C402" s="13" t="s">
         <v>1</v>
@@ -19148,10 +19148,10 @@
     </row>
     <row r="403" spans="1:6">
       <c r="A403" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B403" s="3" t="s">
         <v>597</v>
-      </c>
-      <c r="B403" s="3" t="s">
-        <v>598</v>
       </c>
       <c r="C403" s="13" t="s">
         <v>1</v>
@@ -19168,10 +19168,10 @@
     </row>
     <row r="404" spans="1:6">
       <c r="A404" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="B404" s="3" t="s">
         <v>640</v>
-      </c>
-      <c r="B404" s="3" t="s">
-        <v>641</v>
       </c>
       <c r="C404" s="13" t="s">
         <v>1</v>
@@ -19188,10 +19188,10 @@
     </row>
     <row r="405" spans="1:6">
       <c r="A405" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C405" s="13" t="s">
         <v>1</v>
@@ -19208,10 +19208,10 @@
     </row>
     <row r="406" spans="1:6">
       <c r="A406" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B406" s="3" t="s">
         <v>576</v>
-      </c>
-      <c r="B406" s="3" t="s">
-        <v>577</v>
       </c>
       <c r="C406" s="13" t="s">
         <v>1</v>
@@ -19228,10 +19228,10 @@
     </row>
     <row r="407" spans="1:6">
       <c r="A407" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C407" s="13" t="s">
         <v>1</v>
@@ -19248,10 +19248,10 @@
     </row>
     <row r="408" spans="1:6">
       <c r="A408" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B408" s="3" t="s">
         <v>599</v>
-      </c>
-      <c r="B408" s="3" t="s">
-        <v>600</v>
       </c>
       <c r="C408" s="13" t="s">
         <v>1</v>
@@ -19268,10 +19268,10 @@
     </row>
     <row r="409" spans="1:6">
       <c r="A409" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B409" s="3" t="s">
         <v>618</v>
-      </c>
-      <c r="B409" s="3" t="s">
-        <v>619</v>
       </c>
       <c r="C409" s="13" t="s">
         <v>1</v>
@@ -19288,10 +19288,10 @@
     </row>
     <row r="410" spans="1:6">
       <c r="A410" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C410" s="13" t="s">
         <v>1</v>

</xml_diff>